<commit_message>
Add support for phonetic pronunciation
Add Phoneme_Pronunciation.csv

Allows you to specify exact pronunciation using phonetic alphabets
</commit_message>
<xml_diff>
--- a/SSML_Customization/Examples.xlsx
+++ b/SSML_Customization/Examples.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Dropbox\Programs\My Programs\Auto Translate Dub\SSML_Customization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9AE98F-2ACF-4379-93D0-7FF5451ACCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5300A059-71D9-49D5-92EA-1DB34F0BFD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40900" yWindow="2380" windowWidth="17850" windowHeight="14040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14510" yWindow="5190" windowWidth="17850" windowHeight="14040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="interpret-as" sheetId="1" r:id="rId1"/>
     <sheet name="aliases" sheetId="2" r:id="rId2"/>
     <sheet name="manual translations" sheetId="3" r:id="rId3"/>
+    <sheet name="phoneme pronunciation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Text</t>
   </si>
@@ -162,6 +163,21 @@
   </si>
   <si>
     <t>pl</t>
+  </si>
+  <si>
+    <t>Phonetic Pronunciation</t>
+  </si>
+  <si>
+    <t>Phonetic Alphabet</t>
+  </si>
+  <si>
+    <t>ThioJoe</t>
+  </si>
+  <si>
+    <t>ˈθioʊd͡ʒoʊ</t>
+  </si>
+  <si>
+    <t>ipa</t>
   </si>
 </sst>
 </file>
@@ -624,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6F687-C96A-41A0-8E61-414CE0DB464D}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
@@ -809,4 +825,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B5F5A3-7974-49B8-80A8-176C3A813EF4}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>